<commit_message>
Merged PR 8938: BP1-92 Campaign Export - Contract Tab - Quarterly Delivery - Multiple Spot Lengths
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlansWithDaypartsSorting.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlansWithDaypartsSorting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C4E787E8-1200-41A4-A260-D43CD30914D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E91EEE2-103A-4DE2-B420-4E5455B83C81}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="465" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -225,13 +225,19 @@
     <t>3/15</t>
   </si>
   <si>
+    <t>3/19-20</t>
+  </si>
+  <si>
+    <t>3/28</t>
+  </si>
+  <si>
+    <t>1Q '20 EF :45s</t>
+  </si>
+  <si>
     <t>3/16-17, 3/19-20</t>
   </si>
   <si>
     <t>3/24, 3/28</t>
-  </si>
-  <si>
-    <t>1Q '20 EF :45s</t>
   </si>
   <si>
     <t>1Q '20 EF Total</t>
@@ -273,10 +279,13 @@
     <t>June</t>
   </si>
   <si>
-    <t>4/7, 4/9-11</t>
+    <t>4/9-11</t>
   </si>
   <si>
     <t>2Q '20 EF :45s</t>
+  </si>
+  <si>
+    <t>4/7, 4/9-11</t>
   </si>
   <si>
     <t>2Q '20 EF Total</t>
@@ -814,7 +823,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 03/12/20</t>
+    <t>Created 06/17/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -829,7 +838,7 @@
     <t>A21-24</t>
   </si>
   <si>
-    <t>:45 eq., :45</t>
+    <t>:45, :45 eq.</t>
   </si>
   <si>
     <t>Order</t>
@@ -1292,7 +1301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
@@ -1726,6 +1735,9 @@
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2380,7 +2392,7 @@
   <dimension ref="A2:T78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2405,7 +2417,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/12/20</v>
+        <v>Created 06/17/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -2458,7 +2470,7 @@
       </c>
       <c r="H5" s="76" t="str">
         <f>'PROPOSAL'!L5</f>
-        <v>:45 eq., :45</v>
+        <v>:45, :45 eq.</v>
       </c>
       <c r="I5" s="76" t="str">
         <f>'PROPOSAL'!N5</f>
@@ -2494,7 +2506,7 @@
     </row>
     <row r="7" ht="24" customHeight="1">
       <c r="C7" s="53" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
@@ -2512,19 +2524,19 @@
     </row>
     <row r="8" ht="24" customHeight="1">
       <c r="A8" s="99" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C8" s="86" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D8" s="87" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E8" s="87" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G8" s="87" t="s">
         <v>60</v>
@@ -2533,10 +2545,10 @@
         <v>25</v>
       </c>
       <c r="I8" s="87" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J8" s="92" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K8" s="88" t="s">
         <v>30</v>
@@ -2552,20 +2564,20 @@
     </row>
     <row r="9" ht="24" customHeight="1">
       <c r="A9" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D9" s="82" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E9" s="83">
         <v>0</v>
       </c>
       <c r="F9" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G9" s="85">
         <v>0</v>
@@ -2577,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K9" s="95">
         <v>25</v>
@@ -2585,20 +2597,20 @@
     </row>
     <row r="10" ht="24" customHeight="1">
       <c r="A10" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D10" s="82" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E10" s="83">
         <v>0</v>
       </c>
       <c r="F10" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G10" s="85">
         <v>0</v>
@@ -2610,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K10" s="95">
         <v>25</v>
@@ -2618,20 +2630,20 @@
     </row>
     <row r="11" ht="24" customHeight="1">
       <c r="A11" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="83">
+        <v>0</v>
+      </c>
+      <c r="F11" s="84" t="s">
         <v>104</v>
-      </c>
-      <c r="D11" s="82" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="83">
-        <v>0</v>
-      </c>
-      <c r="F11" s="84" t="s">
-        <v>101</v>
       </c>
       <c r="G11" s="85">
         <v>0</v>
@@ -2643,7 +2655,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K11" s="95">
         <v>25</v>
@@ -2651,20 +2663,20 @@
     </row>
     <row r="12" ht="24" customHeight="1">
       <c r="A12" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="81" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D12" s="82" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E12" s="83">
         <v>0</v>
       </c>
       <c r="F12" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G12" s="85">
         <v>0</v>
@@ -2676,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K12" s="95">
         <v>25</v>
@@ -2684,20 +2696,20 @@
     </row>
     <row r="13" ht="24" customHeight="1">
       <c r="A13" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E13" s="83">
         <v>0</v>
       </c>
       <c r="F13" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G13" s="85">
         <v>0</v>
@@ -2709,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K13" s="95">
         <v>25</v>
@@ -2717,20 +2729,20 @@
     </row>
     <row r="14" ht="24" customHeight="1">
       <c r="A14" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E14" s="83">
         <v>0</v>
       </c>
       <c r="F14" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G14" s="85">
         <v>0</v>
@@ -2742,7 +2754,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K14" s="95">
         <v>25</v>
@@ -2750,20 +2762,20 @@
     </row>
     <row r="15" ht="24" customHeight="1">
       <c r="A15" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E15" s="83">
         <v>0</v>
       </c>
       <c r="F15" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G15" s="85">
         <v>0</v>
@@ -2775,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K15" s="95">
         <v>25</v>
@@ -2783,20 +2795,20 @@
     </row>
     <row r="16" ht="24" customHeight="1">
       <c r="A16" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D16" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="83">
+        <v>0</v>
+      </c>
+      <c r="F16" s="84" t="s">
         <v>106</v>
-      </c>
-      <c r="E16" s="83">
-        <v>0</v>
-      </c>
-      <c r="F16" s="84" t="s">
-        <v>103</v>
       </c>
       <c r="G16" s="85">
         <v>0</v>
@@ -2808,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K16" s="95">
         <v>25</v>
@@ -2816,20 +2828,20 @@
     </row>
     <row r="17" ht="24" customHeight="1">
       <c r="A17" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="83">
+        <v>0</v>
+      </c>
+      <c r="F17" s="84" t="s">
         <v>104</v>
-      </c>
-      <c r="D17" s="82" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="83">
-        <v>0</v>
-      </c>
-      <c r="F17" s="84" t="s">
-        <v>101</v>
       </c>
       <c r="G17" s="85">
         <v>0</v>
@@ -2841,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K17" s="95">
         <v>25</v>
@@ -2849,20 +2861,20 @@
     </row>
     <row r="18" ht="24" customHeight="1">
       <c r="A18" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="81" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D18" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="83">
+        <v>0</v>
+      </c>
+      <c r="F18" s="84" t="s">
         <v>106</v>
-      </c>
-      <c r="E18" s="83">
-        <v>0</v>
-      </c>
-      <c r="F18" s="84" t="s">
-        <v>103</v>
       </c>
       <c r="G18" s="85">
         <v>0</v>
@@ -2874,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K18" s="95">
         <v>25</v>
@@ -2882,20 +2894,20 @@
     </row>
     <row r="19" ht="24" customHeight="1">
       <c r="A19" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D19" s="82" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E19" s="83">
         <v>0</v>
       </c>
       <c r="F19" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G19" s="85">
         <v>0</v>
@@ -2907,7 +2919,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K19" s="95">
         <v>25</v>
@@ -2915,20 +2927,20 @@
     </row>
     <row r="20" ht="24" customHeight="1">
       <c r="A20" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D20" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="83">
+        <v>0</v>
+      </c>
+      <c r="F20" s="84" t="s">
         <v>106</v>
-      </c>
-      <c r="E20" s="83">
-        <v>0</v>
-      </c>
-      <c r="F20" s="84" t="s">
-        <v>103</v>
       </c>
       <c r="G20" s="85">
         <v>0</v>
@@ -2940,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K20" s="95">
         <v>25</v>
@@ -2948,20 +2960,20 @@
     </row>
     <row r="21" ht="24" customHeight="1">
       <c r="A21" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E21" s="83">
         <v>0</v>
       </c>
       <c r="F21" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G21" s="85">
         <v>0</v>
@@ -2973,7 +2985,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K21" s="95">
         <v>25</v>
@@ -2981,20 +2993,20 @@
     </row>
     <row r="22" ht="24" customHeight="1">
       <c r="A22" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D22" s="82" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E22" s="83">
         <v>0</v>
       </c>
       <c r="F22" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G22" s="85">
         <v>0</v>
@@ -3006,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K22" s="95">
         <v>25</v>
@@ -3014,20 +3026,20 @@
     </row>
     <row r="23" ht="24" customHeight="1">
       <c r="A23" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="82" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="83">
+        <v>0</v>
+      </c>
+      <c r="F23" s="84" t="s">
         <v>104</v>
-      </c>
-      <c r="D23" s="82" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="83">
-        <v>0</v>
-      </c>
-      <c r="F23" s="84" t="s">
-        <v>101</v>
       </c>
       <c r="G23" s="85">
         <v>0</v>
@@ -3039,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K23" s="95">
         <v>25</v>
@@ -3047,20 +3059,20 @@
     </row>
     <row r="24" ht="24" customHeight="1">
       <c r="A24" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="81" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D24" s="82" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E24" s="83">
         <v>0</v>
       </c>
       <c r="F24" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G24" s="85">
         <v>0</v>
@@ -3072,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K24" s="95">
         <v>25</v>
@@ -3080,20 +3092,20 @@
     </row>
     <row r="25" ht="24" customHeight="1">
       <c r="A25" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E25" s="83">
         <v>0</v>
       </c>
       <c r="F25" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G25" s="85">
         <v>0</v>
@@ -3105,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K25" s="95">
         <v>25</v>
@@ -3113,20 +3125,20 @@
     </row>
     <row r="26" ht="24" customHeight="1">
       <c r="A26" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D26" s="82" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E26" s="83">
         <v>0</v>
       </c>
       <c r="F26" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G26" s="85">
         <v>0</v>
@@ -3138,7 +3150,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K26" s="95">
         <v>25</v>
@@ -3147,7 +3159,7 @@
     <row r="27" ht="24" customHeight="1">
       <c r="C27" s="39"/>
       <c r="D27" s="91" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E27" s="97">
         <v>0</v>
@@ -3173,7 +3185,7 @@
     </row>
     <row r="29">
       <c r="C29" s="53" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H29" s="30"/>
       <c r="I29" s="30"/>
@@ -3191,19 +3203,19 @@
     </row>
     <row r="30" ht="24" customHeight="1">
       <c r="A30" s="99" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C30" s="86" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D30" s="87" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E30" s="87" t="s">
         <v>23</v>
       </c>
       <c r="F30" s="87" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G30" s="87" t="s">
         <v>60</v>
@@ -3212,10 +3224,10 @@
         <v>25</v>
       </c>
       <c r="I30" s="87" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J30" s="92" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K30" s="88" t="s">
         <v>30</v>
@@ -3231,7 +3243,7 @@
     </row>
     <row r="31" ht="24" customHeight="1">
       <c r="A31" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="81"/>
@@ -3242,27 +3254,27 @@
         <v>1</v>
       </c>
       <c r="F31" s="84" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G31" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H31" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I31" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J31" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K31" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" ht="24" customHeight="1">
       <c r="A32" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="81"/>
@@ -3273,27 +3285,27 @@
         <v>1</v>
       </c>
       <c r="F32" s="84" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G32" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H32" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I32" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J32" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K32" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" ht="24" customHeight="1">
       <c r="A33" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="81"/>
@@ -3304,27 +3316,27 @@
         <v>1</v>
       </c>
       <c r="F33" s="84" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G33" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H33" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I33" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J33" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K33" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" ht="24" customHeight="1">
       <c r="A34" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="81"/>
@@ -3335,27 +3347,27 @@
         <v>1</v>
       </c>
       <c r="F34" s="84" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G34" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H34" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I34" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J34" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K34" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" ht="24" customHeight="1">
       <c r="A35" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="81"/>
@@ -3366,27 +3378,27 @@
         <v>1</v>
       </c>
       <c r="F35" s="84" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G35" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H35" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I35" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J35" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K35" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" ht="24" customHeight="1">
       <c r="A36" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="81"/>
@@ -3397,28 +3409,28 @@
         <v>1</v>
       </c>
       <c r="F36" s="84" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G36" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H36" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I36" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J36" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K36" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" ht="24" customHeight="1">
       <c r="C37" s="39"/>
       <c r="D37" s="91" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E37" s="97">
         <v>6</v>
@@ -3444,7 +3456,7 @@
     </row>
     <row r="39">
       <c r="C39" s="53" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H39" s="30"/>
       <c r="I39" s="30"/>
@@ -3462,19 +3474,19 @@
     </row>
     <row r="40" ht="24" customHeight="1">
       <c r="A40" s="99" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C40" s="86" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D40" s="87" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E40" s="87" t="s">
         <v>23</v>
       </c>
       <c r="F40" s="87" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G40" s="87" t="s">
         <v>60</v>
@@ -3483,10 +3495,10 @@
         <v>25</v>
       </c>
       <c r="I40" s="87" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J40" s="92" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K40" s="88" t="s">
         <v>30</v>
@@ -3502,20 +3514,20 @@
     </row>
     <row r="41" ht="24" customHeight="1">
       <c r="A41" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D41" s="82" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E41" s="83">
         <v>0</v>
       </c>
       <c r="F41" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G41" s="85">
         <v>0</v>
@@ -3527,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K41" s="95">
         <v>25</v>
@@ -3535,20 +3547,20 @@
     </row>
     <row r="42" ht="24" customHeight="1">
       <c r="A42" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D42" s="82" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E42" s="83">
         <v>0</v>
       </c>
       <c r="F42" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G42" s="85">
         <v>0</v>
@@ -3560,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K42" s="95">
         <v>25</v>
@@ -3568,20 +3580,20 @@
     </row>
     <row r="43" ht="24" customHeight="1">
       <c r="A43" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" s="83">
+        <v>0</v>
+      </c>
+      <c r="F43" s="84" t="s">
         <v>104</v>
-      </c>
-      <c r="D43" s="82" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="83">
-        <v>0</v>
-      </c>
-      <c r="F43" s="84" t="s">
-        <v>101</v>
       </c>
       <c r="G43" s="85">
         <v>0</v>
@@ -3593,7 +3605,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K43" s="95">
         <v>25</v>
@@ -3601,20 +3613,20 @@
     </row>
     <row r="44" ht="24" customHeight="1">
       <c r="A44" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="81" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D44" s="82" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E44" s="83">
         <v>0</v>
       </c>
       <c r="F44" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G44" s="85">
         <v>0</v>
@@ -3626,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K44" s="95">
         <v>25</v>
@@ -3634,20 +3646,20 @@
     </row>
     <row r="45" ht="24" customHeight="1">
       <c r="A45" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D45" s="82" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E45" s="83">
         <v>0</v>
       </c>
       <c r="F45" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G45" s="85">
         <v>0</v>
@@ -3659,7 +3671,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K45" s="95">
         <v>25</v>
@@ -3667,20 +3679,20 @@
     </row>
     <row r="46" ht="24" customHeight="1">
       <c r="A46" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D46" s="82" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E46" s="83">
         <v>0</v>
       </c>
       <c r="F46" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G46" s="85">
         <v>0</v>
@@ -3692,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K46" s="95">
         <v>25</v>
@@ -3700,20 +3712,20 @@
     </row>
     <row r="47" ht="24" customHeight="1">
       <c r="A47" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D47" s="82" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E47" s="83">
         <v>0</v>
       </c>
       <c r="F47" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G47" s="85">
         <v>0</v>
@@ -3725,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K47" s="95">
         <v>25</v>
@@ -3733,20 +3745,20 @@
     </row>
     <row r="48" ht="24" customHeight="1">
       <c r="A48" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D48" s="82" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E48" s="83">
         <v>0</v>
       </c>
       <c r="F48" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G48" s="85">
         <v>0</v>
@@ -3758,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="J48" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K48" s="95">
         <v>25</v>
@@ -3766,20 +3778,20 @@
     </row>
     <row r="49" ht="24" customHeight="1">
       <c r="A49" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="83">
+        <v>0</v>
+      </c>
+      <c r="F49" s="84" t="s">
         <v>104</v>
-      </c>
-      <c r="D49" s="82" t="s">
-        <v>113</v>
-      </c>
-      <c r="E49" s="83">
-        <v>0</v>
-      </c>
-      <c r="F49" s="84" t="s">
-        <v>101</v>
       </c>
       <c r="G49" s="85">
         <v>0</v>
@@ -3791,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="J49" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K49" s="95">
         <v>25</v>
@@ -3799,20 +3811,20 @@
     </row>
     <row r="50" ht="24" customHeight="1">
       <c r="A50" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="81" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D50" s="82" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E50" s="83">
         <v>0</v>
       </c>
       <c r="F50" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G50" s="85">
         <v>0</v>
@@ -3824,7 +3836,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="93">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="K50" s="95">
         <v>25</v>
@@ -3832,20 +3844,20 @@
     </row>
     <row r="51" ht="24" customHeight="1">
       <c r="A51" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D51" s="82" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E51" s="83">
         <v>0</v>
       </c>
       <c r="F51" s="84" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G51" s="85">
         <v>0</v>
@@ -3857,7 +3869,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K51" s="95">
         <v>25</v>
@@ -3865,20 +3877,20 @@
     </row>
     <row r="52" ht="24" customHeight="1">
       <c r="A52" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D52" s="82" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E52" s="83">
         <v>0</v>
       </c>
       <c r="F52" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G52" s="85">
         <v>0</v>
@@ -3890,7 +3902,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="93">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="K52" s="95">
         <v>25</v>
@@ -3899,7 +3911,7 @@
     <row r="53" ht="24" customHeight="1">
       <c r="C53" s="39"/>
       <c r="D53" s="91" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E53" s="97">
         <v>0</v>
@@ -3925,7 +3937,7 @@
     </row>
     <row r="55">
       <c r="C55" s="53" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H55" s="30"/>
       <c r="I55" s="30"/>
@@ -3943,19 +3955,19 @@
     </row>
     <row r="56" ht="24" customHeight="1">
       <c r="A56" s="99" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C56" s="86" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D56" s="87" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E56" s="87" t="s">
         <v>23</v>
       </c>
       <c r="F56" s="87" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G56" s="87" t="s">
         <v>60</v>
@@ -3964,10 +3976,10 @@
         <v>25</v>
       </c>
       <c r="I56" s="87" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J56" s="92" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K56" s="88" t="s">
         <v>30</v>
@@ -3983,7 +3995,7 @@
     </row>
     <row r="57" ht="24" customHeight="1">
       <c r="A57" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="81"/>
@@ -3994,27 +4006,27 @@
         <v>1</v>
       </c>
       <c r="F57" s="84" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G57" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H57" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I57" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J57" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K57" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" ht="24" customHeight="1">
       <c r="A58" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="81"/>
@@ -4025,27 +4037,27 @@
         <v>1</v>
       </c>
       <c r="F58" s="84" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G58" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H58" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I58" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J58" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K58" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" ht="24" customHeight="1">
       <c r="A59" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="81"/>
@@ -4056,27 +4068,27 @@
         <v>1</v>
       </c>
       <c r="F59" s="84" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G59" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H59" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I59" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J59" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K59" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" ht="24" customHeight="1">
       <c r="A60" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="81"/>
@@ -4087,28 +4099,28 @@
         <v>1</v>
       </c>
       <c r="F60" s="84" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G60" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H60" s="85" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I60" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J60" s="93" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K60" s="95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" ht="24" customHeight="1">
       <c r="C61" s="39"/>
       <c r="D61" s="91" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E61" s="97">
         <v>4</v>
@@ -4134,7 +4146,7 @@
     </row>
     <row r="63" ht="24" customHeight="1">
       <c r="C63" s="53" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I63" s="60"/>
     </row>
@@ -4147,7 +4159,7 @@
       </c>
       <c r="E64" s="101"/>
       <c r="F64" s="101" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G64" s="101"/>
       <c r="H64" s="101" t="s">
@@ -4183,13 +4195,13 @@
     </row>
     <row r="67" ht="24" customHeight="1">
       <c r="C67" s="113" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D67" s="109"/>
       <c r="E67" s="109"/>
       <c r="F67" s="112"/>
       <c r="G67" s="114" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H67" s="109"/>
       <c r="I67" s="115"/>
@@ -4208,7 +4220,7 @@
         <v>42</v>
       </c>
       <c r="D69" s="136" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E69" s="136"/>
       <c r="F69" s="136"/>
@@ -4326,7 +4338,7 @@
         <v>49</v>
       </c>
       <c r="D75" s="136" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E75" s="136"/>
       <c r="F75" s="136"/>
@@ -4366,7 +4378,7 @@
         <v>51</v>
       </c>
       <c r="D77" s="136" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E77" s="136"/>
       <c r="F77" s="136"/>
@@ -4471,7 +4483,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/12/20</v>
+        <v>Created 06/17/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -4515,7 +4527,7 @@
       <c r="P6" s="60"/>
     </row>
     <row r="7">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="146" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="138" t="s">
@@ -4713,16 +4725,16 @@
         <v>0</v>
       </c>
       <c r="M11" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="N11" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="O11" s="58">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="P11" s="58">
-        <v>4800.0000000000009</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="12" ht="24" customHeight="1">
@@ -4843,11 +4855,11 @@
         <v>64</v>
       </c>
       <c r="P14" s="130">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="146" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="138" t="s">
@@ -5045,16 +5057,16 @@
         <v>0</v>
       </c>
       <c r="M20" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="N20" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="O20" s="58">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="P20" s="58">
-        <v>4800.0000000000009</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="21" ht="24" customHeight="1">
@@ -5169,18 +5181,18 @@
         <v>62</v>
       </c>
       <c r="N23" s="132" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O23" s="133" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P23" s="130">
         <v>7</v>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="53" t="s">
-        <v>66</v>
+      <c r="B25" s="146" t="s">
+        <v>68</v>
       </c>
       <c r="C25" s="138" t="s">
         <v>56</v>
@@ -5377,16 +5389,16 @@
         <v>0</v>
       </c>
       <c r="M29" s="36">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="N29" s="36">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="O29" s="58">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="P29" s="58">
-        <v>9600.0000000000018</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="30" ht="24" customHeight="1">
@@ -5501,18 +5513,18 @@
         <v>62</v>
       </c>
       <c r="N32" s="132" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O32" s="133" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P32" s="130">
         <v>7</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="53" t="s">
-        <v>67</v>
+      <c r="B34" s="146" t="s">
+        <v>69</v>
       </c>
       <c r="C34" s="138" t="s">
         <v>56</v>
@@ -5709,16 +5721,16 @@
         <v>0</v>
       </c>
       <c r="M38" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="N38" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="O38" s="58">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="P38" s="58">
-        <v>4800.0000000000009</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="39" ht="24" customHeight="1">
@@ -5839,12 +5851,12 @@
         <v>64</v>
       </c>
       <c r="P41" s="130">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="53" t="s">
-        <v>68</v>
+      <c r="B43" s="146" t="s">
+        <v>70</v>
       </c>
       <c r="C43" s="138" t="s">
         <v>56</v>
@@ -6041,16 +6053,16 @@
         <v>0</v>
       </c>
       <c r="M47" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="N47" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="O47" s="58">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="P47" s="58">
-        <v>4800.0000000000009</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="48" ht="24" customHeight="1">
@@ -6165,18 +6177,18 @@
         <v>62</v>
       </c>
       <c r="N50" s="132" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O50" s="133" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P50" s="130">
         <v>7</v>
       </c>
     </row>
     <row r="52">
-      <c r="B52" s="53" t="s">
-        <v>69</v>
+      <c r="B52" s="146" t="s">
+        <v>71</v>
       </c>
       <c r="C52" s="138" t="s">
         <v>56</v>
@@ -6373,16 +6385,16 @@
         <v>0</v>
       </c>
       <c r="M56" s="36">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="N56" s="36">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="O56" s="58">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="P56" s="58">
-        <v>9600.0000000000018</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="57" ht="24" customHeight="1">
@@ -6497,18 +6509,18 @@
         <v>62</v>
       </c>
       <c r="N59" s="132" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O59" s="133" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P59" s="130">
         <v>7</v>
       </c>
     </row>
     <row r="61">
-      <c r="B61" s="53" t="s">
-        <v>70</v>
+      <c r="B61" s="146" t="s">
+        <v>72</v>
       </c>
       <c r="C61" s="138" t="s">
         <v>56</v>
@@ -6705,16 +6717,16 @@
         <v>0</v>
       </c>
       <c r="M65" s="36">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="N65" s="36">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="O65" s="58">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="P65" s="58">
-        <v>2400.0000000000005</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="66" ht="24" customHeight="1">
@@ -6835,12 +6847,12 @@
         <v>64</v>
       </c>
       <c r="P68" s="130">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
-      <c r="B70" s="53" t="s">
-        <v>71</v>
+      <c r="B70" s="146" t="s">
+        <v>73</v>
       </c>
       <c r="C70" s="138" t="s">
         <v>56</v>
@@ -7037,16 +7049,16 @@
         <v>0</v>
       </c>
       <c r="M74" s="36">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="N74" s="36">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="O74" s="58">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="P74" s="58">
-        <v>2400.0000000000005</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="75" ht="24" customHeight="1">
@@ -7161,18 +7173,18 @@
         <v>62</v>
       </c>
       <c r="N77" s="132" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O77" s="133" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P77" s="130">
         <v>7</v>
       </c>
     </row>
     <row r="79">
-      <c r="B79" s="53" t="s">
-        <v>72</v>
+      <c r="B79" s="146" t="s">
+        <v>74</v>
       </c>
       <c r="C79" s="138" t="s">
         <v>56</v>
@@ -7369,16 +7381,16 @@
         <v>0</v>
       </c>
       <c r="M83" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="N83" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="O83" s="58">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="P83" s="58">
-        <v>4800.0000000000009</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="84" ht="24" customHeight="1">
@@ -7493,18 +7505,18 @@
         <v>62</v>
       </c>
       <c r="N86" s="132" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O86" s="133" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P86" s="130">
         <v>7</v>
       </c>
     </row>
     <row r="88">
-      <c r="B88" s="53" t="s">
-        <v>73</v>
+      <c r="B88" s="146" t="s">
+        <v>75</v>
       </c>
       <c r="C88" s="138" t="s">
         <v>56</v>
@@ -7635,16 +7647,16 @@
       <c r="K92" s="66"/>
       <c r="L92" s="36"/>
       <c r="M92" s="36" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N92" s="36" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O92" s="58" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P92" s="58" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" ht="24" customHeight="1">
@@ -7662,16 +7674,16 @@
       <c r="K93" s="73"/>
       <c r="L93" s="38"/>
       <c r="M93" s="38" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N93" s="38" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O93" s="74" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P93" s="74" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="94" ht="24" customHeight="1">
@@ -7689,16 +7701,16 @@
       <c r="K94" s="70"/>
       <c r="L94" s="71"/>
       <c r="M94" s="71" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N94" s="71" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O94" s="72" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P94" s="72" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="95" ht="30" customHeight="1">
@@ -7719,34 +7731,34 @@
         <v>62</v>
       </c>
       <c r="N95" s="132" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O95" s="133" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P95" s="130">
         <v>7</v>
       </c>
     </row>
     <row r="97">
-      <c r="B97" s="53" t="s">
-        <v>75</v>
+      <c r="B97" s="146" t="s">
+        <v>77</v>
       </c>
       <c r="C97" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D97" s="139"/>
       <c r="E97" s="139"/>
       <c r="F97" s="140"/>
       <c r="G97" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H97" s="139"/>
       <c r="I97" s="139"/>
       <c r="J97" s="139"/>
       <c r="K97" s="140"/>
       <c r="L97" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M97" s="139"/>
       <c r="N97" s="139"/>
@@ -7897,10 +7909,10 @@
         <v>28</v>
       </c>
       <c r="C101" s="66">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="D101" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="E101" s="36">
         <v>0</v>
@@ -7936,7 +7948,7 @@
         <v>0</v>
       </c>
       <c r="P101" s="58">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="102" ht="24" customHeight="1">
@@ -8039,7 +8051,7 @@
       </c>
       <c r="C104" s="131"/>
       <c r="D104" s="132" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E104" s="132"/>
       <c r="F104" s="132"/>
@@ -8053,28 +8065,28 @@
       <c r="N104" s="132"/>
       <c r="O104" s="133"/>
       <c r="P104" s="130">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106">
-      <c r="B106" s="53" t="s">
-        <v>80</v>
+      <c r="B106" s="146" t="s">
+        <v>82</v>
       </c>
       <c r="C106" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D106" s="139"/>
       <c r="E106" s="139"/>
       <c r="F106" s="140"/>
       <c r="G106" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H106" s="139"/>
       <c r="I106" s="139"/>
       <c r="J106" s="139"/>
       <c r="K106" s="140"/>
       <c r="L106" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M106" s="139"/>
       <c r="N106" s="139"/>
@@ -8225,10 +8237,10 @@
         <v>28</v>
       </c>
       <c r="C110" s="66">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="D110" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="E110" s="36">
         <v>0</v>
@@ -8264,7 +8276,7 @@
         <v>0</v>
       </c>
       <c r="P110" s="58">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="111" ht="24" customHeight="1">
@@ -8367,7 +8379,7 @@
       </c>
       <c r="C113" s="131"/>
       <c r="D113" s="132" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E113" s="132"/>
       <c r="F113" s="132"/>
@@ -8385,24 +8397,24 @@
       </c>
     </row>
     <row r="115">
-      <c r="B115" s="53" t="s">
-        <v>81</v>
+      <c r="B115" s="146" t="s">
+        <v>84</v>
       </c>
       <c r="C115" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D115" s="139"/>
       <c r="E115" s="139"/>
       <c r="F115" s="140"/>
       <c r="G115" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H115" s="139"/>
       <c r="I115" s="139"/>
       <c r="J115" s="139"/>
       <c r="K115" s="140"/>
       <c r="L115" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M115" s="139"/>
       <c r="N115" s="139"/>
@@ -8553,10 +8565,10 @@
         <v>28</v>
       </c>
       <c r="C119" s="66">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="D119" s="36">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="E119" s="36">
         <v>0</v>
@@ -8592,7 +8604,7 @@
         <v>0</v>
       </c>
       <c r="P119" s="58">
-        <v>6400.0000000000009</v>
+        <v>6400</v>
       </c>
     </row>
     <row r="120" ht="24" customHeight="1">
@@ -8695,7 +8707,7 @@
       </c>
       <c r="C122" s="131"/>
       <c r="D122" s="132" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E122" s="132"/>
       <c r="F122" s="132"/>
@@ -8713,24 +8725,24 @@
       </c>
     </row>
     <row r="124">
-      <c r="B124" s="53" t="s">
-        <v>82</v>
+      <c r="B124" s="146" t="s">
+        <v>85</v>
       </c>
       <c r="C124" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D124" s="139"/>
       <c r="E124" s="139"/>
       <c r="F124" s="140"/>
       <c r="G124" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H124" s="139"/>
       <c r="I124" s="139"/>
       <c r="J124" s="139"/>
       <c r="K124" s="140"/>
       <c r="L124" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M124" s="139"/>
       <c r="N124" s="139"/>
@@ -8881,10 +8893,10 @@
         <v>28</v>
       </c>
       <c r="C128" s="66">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="D128" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="E128" s="36">
         <v>0</v>
@@ -8920,7 +8932,7 @@
         <v>0</v>
       </c>
       <c r="P128" s="58">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="129" ht="24" customHeight="1">
@@ -9023,7 +9035,7 @@
       </c>
       <c r="C131" s="131"/>
       <c r="D131" s="132" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E131" s="132"/>
       <c r="F131" s="132"/>
@@ -9037,28 +9049,28 @@
       <c r="N131" s="132"/>
       <c r="O131" s="133"/>
       <c r="P131" s="130">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
-      <c r="B133" s="53" t="s">
-        <v>83</v>
+      <c r="B133" s="146" t="s">
+        <v>86</v>
       </c>
       <c r="C133" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D133" s="139"/>
       <c r="E133" s="139"/>
       <c r="F133" s="140"/>
       <c r="G133" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H133" s="139"/>
       <c r="I133" s="139"/>
       <c r="J133" s="139"/>
       <c r="K133" s="140"/>
       <c r="L133" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M133" s="139"/>
       <c r="N133" s="139"/>
@@ -9209,10 +9221,10 @@
         <v>28</v>
       </c>
       <c r="C137" s="66">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="D137" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="E137" s="36">
         <v>0</v>
@@ -9248,7 +9260,7 @@
         <v>0</v>
       </c>
       <c r="P137" s="58">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="138" ht="24" customHeight="1">
@@ -9351,7 +9363,7 @@
       </c>
       <c r="C140" s="131"/>
       <c r="D140" s="132" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E140" s="132"/>
       <c r="F140" s="132"/>
@@ -9369,24 +9381,24 @@
       </c>
     </row>
     <row r="142">
-      <c r="B142" s="53" t="s">
-        <v>84</v>
+      <c r="B142" s="146" t="s">
+        <v>87</v>
       </c>
       <c r="C142" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D142" s="139"/>
       <c r="E142" s="139"/>
       <c r="F142" s="140"/>
       <c r="G142" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H142" s="139"/>
       <c r="I142" s="139"/>
       <c r="J142" s="139"/>
       <c r="K142" s="140"/>
       <c r="L142" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M142" s="139"/>
       <c r="N142" s="139"/>
@@ -9537,10 +9549,10 @@
         <v>28</v>
       </c>
       <c r="C146" s="66">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="D146" s="36">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="E146" s="36">
         <v>0</v>
@@ -9576,7 +9588,7 @@
         <v>0</v>
       </c>
       <c r="P146" s="58">
-        <v>6400.0000000000009</v>
+        <v>6400</v>
       </c>
     </row>
     <row r="147" ht="24" customHeight="1">
@@ -9679,7 +9691,7 @@
       </c>
       <c r="C149" s="131"/>
       <c r="D149" s="132" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E149" s="132"/>
       <c r="F149" s="132"/>
@@ -9697,24 +9709,24 @@
       </c>
     </row>
     <row r="151">
-      <c r="B151" s="53" t="s">
-        <v>85</v>
+      <c r="B151" s="146" t="s">
+        <v>88</v>
       </c>
       <c r="C151" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D151" s="139"/>
       <c r="E151" s="139"/>
       <c r="F151" s="140"/>
       <c r="G151" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H151" s="139"/>
       <c r="I151" s="139"/>
       <c r="J151" s="139"/>
       <c r="K151" s="140"/>
       <c r="L151" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M151" s="139"/>
       <c r="N151" s="139"/>
@@ -9865,10 +9877,10 @@
         <v>28</v>
       </c>
       <c r="C155" s="66">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="D155" s="36">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="E155" s="36">
         <v>0</v>
@@ -9904,7 +9916,7 @@
         <v>0</v>
       </c>
       <c r="P155" s="58">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="156" ht="24" customHeight="1">
@@ -10007,7 +10019,7 @@
       </c>
       <c r="C158" s="131"/>
       <c r="D158" s="132" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E158" s="132"/>
       <c r="F158" s="132"/>
@@ -10021,28 +10033,28 @@
       <c r="N158" s="132"/>
       <c r="O158" s="133"/>
       <c r="P158" s="130">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160">
-      <c r="B160" s="53" t="s">
-        <v>86</v>
+      <c r="B160" s="146" t="s">
+        <v>89</v>
       </c>
       <c r="C160" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D160" s="139"/>
       <c r="E160" s="139"/>
       <c r="F160" s="140"/>
       <c r="G160" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H160" s="139"/>
       <c r="I160" s="139"/>
       <c r="J160" s="139"/>
       <c r="K160" s="140"/>
       <c r="L160" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M160" s="139"/>
       <c r="N160" s="139"/>
@@ -10193,10 +10205,10 @@
         <v>28</v>
       </c>
       <c r="C164" s="66">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="D164" s="36">
-        <v>800.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="E164" s="36">
         <v>0</v>
@@ -10232,7 +10244,7 @@
         <v>0</v>
       </c>
       <c r="P164" s="58">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="165" ht="24" customHeight="1">
@@ -10335,7 +10347,7 @@
       </c>
       <c r="C167" s="131"/>
       <c r="D167" s="132" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E167" s="132"/>
       <c r="F167" s="132"/>
@@ -10353,24 +10365,24 @@
       </c>
     </row>
     <row r="169">
-      <c r="B169" s="53" t="s">
-        <v>87</v>
+      <c r="B169" s="146" t="s">
+        <v>90</v>
       </c>
       <c r="C169" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D169" s="139"/>
       <c r="E169" s="139"/>
       <c r="F169" s="140"/>
       <c r="G169" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H169" s="139"/>
       <c r="I169" s="139"/>
       <c r="J169" s="139"/>
       <c r="K169" s="140"/>
       <c r="L169" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M169" s="139"/>
       <c r="N169" s="139"/>
@@ -10521,10 +10533,10 @@
         <v>28</v>
       </c>
       <c r="C173" s="66">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="D173" s="36">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="E173" s="36">
         <v>0</v>
@@ -10560,7 +10572,7 @@
         <v>0</v>
       </c>
       <c r="P173" s="58">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="174" ht="24" customHeight="1">
@@ -10663,7 +10675,7 @@
       </c>
       <c r="C176" s="131"/>
       <c r="D176" s="132" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E176" s="132"/>
       <c r="F176" s="132"/>
@@ -10681,24 +10693,24 @@
       </c>
     </row>
     <row r="178">
-      <c r="B178" s="53" t="s">
-        <v>88</v>
+      <c r="B178" s="146" t="s">
+        <v>91</v>
       </c>
       <c r="C178" s="138" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D178" s="139"/>
       <c r="E178" s="139"/>
       <c r="F178" s="140"/>
       <c r="G178" s="139" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H178" s="139"/>
       <c r="I178" s="139"/>
       <c r="J178" s="139"/>
       <c r="K178" s="140"/>
       <c r="L178" s="138" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M178" s="139"/>
       <c r="N178" s="139"/>
@@ -10801,10 +10813,10 @@
         <v>28</v>
       </c>
       <c r="C182" s="66" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D182" s="36" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E182" s="36"/>
       <c r="F182" s="58"/>
@@ -10818,7 +10830,7 @@
       <c r="N182" s="36"/>
       <c r="O182" s="58"/>
       <c r="P182" s="58" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="183" ht="24" customHeight="1">
@@ -10826,10 +10838,10 @@
         <v>30</v>
       </c>
       <c r="C183" s="73" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D183" s="38" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E183" s="38"/>
       <c r="F183" s="74"/>
@@ -10843,7 +10855,7 @@
       <c r="N183" s="38"/>
       <c r="O183" s="74"/>
       <c r="P183" s="74" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="184" ht="24" customHeight="1">
@@ -10851,10 +10863,10 @@
         <v>60</v>
       </c>
       <c r="C184" s="70" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D184" s="71" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E184" s="71"/>
       <c r="F184" s="72"/>
@@ -10868,7 +10880,7 @@
       <c r="N184" s="71"/>
       <c r="O184" s="72"/>
       <c r="P184" s="72" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="185" ht="30" customHeight="1">
@@ -10877,7 +10889,7 @@
       </c>
       <c r="C185" s="131"/>
       <c r="D185" s="132" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E185" s="132"/>
       <c r="F185" s="132"/>
@@ -11064,7 +11076,7 @@
         <v>14</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>16</v>
@@ -11097,7 +11109,7 @@
     </row>
     <row r="7" ht="24" customHeight="1">
       <c r="B7" s="53" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -11358,7 +11370,7 @@
     </row>
     <row r="13" ht="24" customHeight="1">
       <c r="B13" s="53" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -13566,11 +13578,6 @@
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -13580,6 +13587,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -13614,97 +13626,97 @@
     <row r="1" ht="18" customHeight="1"/>
     <row r="2" ht="27.95" customHeight="1">
       <c r="D2" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
     <row r="4" ht="104.1" customHeight="1" s="116" customFormat="1">
       <c r="C4" s="144" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D4" s="144"/>
     </row>
     <row r="5" ht="110.1" customHeight="1" s="116" customFormat="1">
       <c r="C5" s="144" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D5" s="144"/>
     </row>
     <row r="6" ht="209.1" customHeight="1" s="116" customFormat="1">
       <c r="C6" s="144" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D6" s="144"/>
     </row>
     <row r="7" ht="89.1" customHeight="1" s="116" customFormat="1">
       <c r="C7" s="144" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D7" s="144"/>
     </row>
     <row r="8" ht="150" customHeight="1" s="116" customFormat="1">
       <c r="C8" s="144" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D8" s="144"/>
     </row>
     <row r="9" ht="200.1" customHeight="1" s="116" customFormat="1">
       <c r="C9" s="144" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D9" s="144"/>
     </row>
     <row r="10" ht="147.95" customHeight="1" s="116" customFormat="1">
       <c r="C10" s="144" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D10" s="144"/>
     </row>
     <row r="11" ht="134.1" customHeight="1" s="116" customFormat="1">
       <c r="C11" s="144" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D11" s="144"/>
     </row>
     <row r="12" ht="54" customHeight="1" s="116" customFormat="1">
       <c r="C12" s="144" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D12" s="144"/>
     </row>
     <row r="13" ht="69.95" customHeight="1" s="116" customFormat="1">
       <c r="C13" s="144" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D13" s="144"/>
     </row>
     <row r="14" ht="128.1" customHeight="1" s="116" customFormat="1">
       <c r="C14" s="144" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D14" s="144"/>
     </row>
     <row r="15" ht="51.95" customHeight="1" s="116" customFormat="1">
       <c r="C15" s="144" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D15" s="144"/>
     </row>
     <row r="16" ht="84" customHeight="1" s="116" customFormat="1">
       <c r="C16" s="144" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D16" s="144"/>
     </row>
     <row r="17" ht="69.95" customHeight="1" s="116" customFormat="1">
       <c r="C17" s="144" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D17" s="144"/>
     </row>
     <row r="18" ht="180" customHeight="1" s="116" customFormat="1">
       <c r="C18" s="144" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D18" s="144"/>
     </row>
@@ -13765,10 +13777,10 @@
     <row r="2" ht="27.95" customHeight="1">
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -13803,24 +13815,24 @@
     </row>
     <row r="5" ht="18" customHeight="1" s="3" customFormat="1">
       <c r="C5" s="134" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D5" s="134"/>
       <c r="E5" s="134" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F5" s="134"/>
       <c r="G5" s="134"/>
       <c r="H5" s="134" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="I5" s="134"/>
       <c r="J5" s="134" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="K5" s="134"/>
       <c r="L5" s="134" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="M5" s="134"/>
       <c r="N5" s="76" t="s">
@@ -13832,7 +13844,7 @@
       <c r="R5" s="134"/>
       <c r="S5" s="134"/>
       <c r="T5" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" ht="18" customHeight="1">
@@ -13852,7 +13864,7 @@
     </row>
     <row r="7" ht="24" customHeight="1">
       <c r="C7" s="53" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D7" s="53"/>
       <c r="E7" s="7"/>
@@ -13867,7 +13879,7 @@
       <c r="L7" s="139"/>
       <c r="M7" s="140"/>
       <c r="N7" s="138" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="O7" s="139"/>
       <c r="P7" s="139"/>
@@ -13878,14 +13890,14 @@
     </row>
     <row r="8" ht="24" customHeight="1">
       <c r="A8" s="99" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E8" s="40" t="s">
         <v>23</v>
@@ -13938,14 +13950,14 @@
     </row>
     <row r="9" ht="24" customHeight="1">
       <c r="A9" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E9" s="119">
         <v>0</v>
@@ -13960,7 +13972,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="123">
-        <v>8.7100015859461219</v>
+        <v>7.9440000000000008</v>
       </c>
       <c r="J9" s="119">
         <v>0</v>
@@ -13972,7 +13984,7 @@
         <v>12.5</v>
       </c>
       <c r="M9" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N9" s="125">
         <v>0.5</v>
@@ -13981,7 +13993,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="123">
-        <v>35.867040879459836</v>
+        <v>30</v>
       </c>
       <c r="Q9" s="119">
         <v>0</v>
@@ -13993,19 +14005,19 @@
         <v>25</v>
       </c>
       <c r="T9" s="121">
-        <v>3345.6900000000041</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="10" ht="24" customHeight="1">
       <c r="A10" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E10" s="119">
         <v>0</v>
@@ -14020,7 +14032,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="123">
-        <v>8.7100015859461219</v>
+        <v>7.9440000000000008</v>
       </c>
       <c r="J10" s="119">
         <v>0</v>
@@ -14032,7 +14044,7 @@
         <v>12.5</v>
       </c>
       <c r="M10" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N10" s="125">
         <v>0.5</v>
@@ -14041,7 +14053,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="123">
-        <v>35.867040879459836</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="119">
         <v>0</v>
@@ -14053,19 +14065,19 @@
         <v>25</v>
       </c>
       <c r="T10" s="121">
-        <v>3345.6900000000041</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="11" ht="24" customHeight="1">
       <c r="A11" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E11" s="119">
         <v>0</v>
@@ -14074,25 +14086,25 @@
         <v>0</v>
       </c>
       <c r="G11" s="121">
-        <v>60000</v>
+        <v>120000</v>
       </c>
       <c r="H11" s="122">
         <v>0</v>
       </c>
       <c r="I11" s="123">
-        <v>4.355000792973061</v>
+        <v>7.9440000000000008</v>
       </c>
       <c r="J11" s="119">
         <v>0</v>
       </c>
       <c r="K11" s="119">
-        <v>4800</v>
+        <v>9600</v>
       </c>
       <c r="L11" s="124">
         <v>12.5</v>
       </c>
       <c r="M11" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N11" s="125">
         <v>0.5</v>
@@ -14101,31 +14113,31 @@
         <v>0</v>
       </c>
       <c r="P11" s="123">
-        <v>17.933520439729918</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="119">
         <v>0</v>
       </c>
       <c r="R11" s="119">
-        <v>2400</v>
+        <v>4800</v>
       </c>
       <c r="S11" s="124">
         <v>25</v>
       </c>
       <c r="T11" s="121">
-        <v>3345.6900000000041</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="12" ht="24" customHeight="1">
       <c r="A12" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="8" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E12" s="119">
         <v>0</v>
@@ -14140,7 +14152,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="123">
-        <v>7.9601990049751246</v>
+        <v>7.9440000000000008</v>
       </c>
       <c r="J12" s="119">
         <v>0</v>
@@ -14152,7 +14164,7 @@
         <v>12.5</v>
       </c>
       <c r="M12" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N12" s="125">
         <v>0.5</v>
@@ -14161,7 +14173,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="123">
-        <v>35.867040879459836</v>
+        <v>30</v>
       </c>
       <c r="Q12" s="119">
         <v>0</v>
@@ -14173,19 +14185,19 @@
         <v>25</v>
       </c>
       <c r="T12" s="121">
-        <v>3345.6900000000041</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="13" ht="24" customHeight="1">
       <c r="A13" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E13" s="119">
         <v>0</v>
@@ -14194,25 +14206,25 @@
         <v>0</v>
       </c>
       <c r="G13" s="121">
-        <v>120000</v>
+        <v>60000</v>
       </c>
       <c r="H13" s="122">
         <v>0</v>
       </c>
       <c r="I13" s="123">
-        <v>7.9601990049751246</v>
+        <v>3.9720000000000004</v>
       </c>
       <c r="J13" s="119">
         <v>0</v>
       </c>
       <c r="K13" s="119">
-        <v>9600</v>
+        <v>4800</v>
       </c>
       <c r="L13" s="124">
         <v>12.5</v>
       </c>
       <c r="M13" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N13" s="125">
         <v>0.5</v>
@@ -14221,31 +14233,31 @@
         <v>0</v>
       </c>
       <c r="P13" s="123">
-        <v>35.867040879459836</v>
+        <v>15</v>
       </c>
       <c r="Q13" s="119">
         <v>0</v>
       </c>
       <c r="R13" s="119">
-        <v>4800</v>
+        <v>2400</v>
       </c>
       <c r="S13" s="124">
         <v>25</v>
       </c>
       <c r="T13" s="121">
-        <v>3345.6900000000041</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="14" ht="24" customHeight="1">
       <c r="A14" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E14" s="119">
         <v>0</v>
@@ -14260,7 +14272,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="123">
-        <v>3.9800995024875623</v>
+        <v>3.9720000000000004</v>
       </c>
       <c r="J14" s="119">
         <v>0</v>
@@ -14272,7 +14284,7 @@
         <v>12.5</v>
       </c>
       <c r="M14" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N14" s="125">
         <v>0.5</v>
@@ -14281,7 +14293,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="123">
-        <v>17.933520439729918</v>
+        <v>15</v>
       </c>
       <c r="Q14" s="119">
         <v>0</v>
@@ -14293,14 +14305,14 @@
         <v>25</v>
       </c>
       <c r="T14" s="121">
-        <v>3345.6900000000041</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="15" ht="24" customHeight="1">
       <c r="B15" s="25"/>
       <c r="C15" s="39"/>
       <c r="D15" s="40" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E15" s="51">
         <v>0</v>
@@ -14315,7 +14327,7 @@
         <v>38</v>
       </c>
       <c r="I15" s="80">
-        <v>41.675501477303115</v>
+        <v>39.720000000000006</v>
       </c>
       <c r="J15" s="51" t="s">
         <v>38</v>
@@ -14327,7 +14339,7 @@
         <v>12.5</v>
       </c>
       <c r="M15" s="43">
-        <v>14396.947336716898</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N15" s="45" t="s">
         <v>38</v>
@@ -14336,7 +14348,7 @@
         <v>38</v>
       </c>
       <c r="P15" s="80">
-        <v>179.33520439729921</v>
+        <v>150</v>
       </c>
       <c r="Q15" s="51" t="s">
         <v>38</v>
@@ -14348,12 +14360,12 @@
         <v>25</v>
       </c>
       <c r="T15" s="43">
-        <v>3345.6900000000041</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="17" ht="24" customHeight="1">
       <c r="C17" s="53" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D17" s="53"/>
       <c r="E17" s="7"/>
@@ -14368,7 +14380,7 @@
       <c r="L17" s="139"/>
       <c r="M17" s="140"/>
       <c r="N17" s="138" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="O17" s="139"/>
       <c r="P17" s="139"/>
@@ -14379,14 +14391,14 @@
     </row>
     <row r="18" ht="24" customHeight="1">
       <c r="A18" s="99" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>23</v>
@@ -14439,14 +14451,14 @@
     </row>
     <row r="19" ht="24" customHeight="1">
       <c r="A19" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E19" s="119">
         <v>0</v>
@@ -14461,19 +14473,19 @@
         <v>0</v>
       </c>
       <c r="I19" s="123">
-        <v>5.8066677239640834</v>
+        <v>5.296</v>
       </c>
       <c r="J19" s="119">
         <v>0</v>
       </c>
       <c r="K19" s="119">
-        <v>6400.0000000000009</v>
+        <v>6400</v>
       </c>
       <c r="L19" s="124">
         <v>12.5</v>
       </c>
       <c r="M19" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N19" s="125">
         <v>0.5</v>
@@ -14482,31 +14494,31 @@
         <v>0</v>
       </c>
       <c r="P19" s="123">
-        <v>23.911360586306564</v>
+        <v>20</v>
       </c>
       <c r="Q19" s="119">
         <v>0</v>
       </c>
       <c r="R19" s="119">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="S19" s="124">
         <v>25</v>
       </c>
       <c r="T19" s="121">
-        <v>3345.6899999999946</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="20" ht="24" customHeight="1">
       <c r="A20" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E20" s="119">
         <v>0</v>
@@ -14521,19 +14533,19 @@
         <v>0</v>
       </c>
       <c r="I20" s="123">
-        <v>5.8066677239640834</v>
+        <v>5.296</v>
       </c>
       <c r="J20" s="119">
         <v>0</v>
       </c>
       <c r="K20" s="119">
-        <v>6400.0000000000009</v>
+        <v>6400</v>
       </c>
       <c r="L20" s="124">
         <v>12.5</v>
       </c>
       <c r="M20" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N20" s="125">
         <v>0.5</v>
@@ -14542,31 +14554,31 @@
         <v>0</v>
       </c>
       <c r="P20" s="123">
-        <v>23.911360586306564</v>
+        <v>20</v>
       </c>
       <c r="Q20" s="119">
         <v>0</v>
       </c>
       <c r="R20" s="119">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="S20" s="124">
         <v>25</v>
       </c>
       <c r="T20" s="121">
-        <v>3345.6899999999946</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="21" ht="24" customHeight="1">
       <c r="A21" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E21" s="119">
         <v>0</v>
@@ -14575,25 +14587,25 @@
         <v>0</v>
       </c>
       <c r="G21" s="121">
-        <v>40000</v>
+        <v>80000</v>
       </c>
       <c r="H21" s="122">
         <v>0</v>
       </c>
       <c r="I21" s="123">
-        <v>2.9033338619820417</v>
+        <v>5.296</v>
       </c>
       <c r="J21" s="119">
         <v>0</v>
       </c>
       <c r="K21" s="119">
-        <v>3200.0000000000005</v>
+        <v>6400</v>
       </c>
       <c r="L21" s="124">
         <v>12.5</v>
       </c>
       <c r="M21" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N21" s="125">
         <v>0.5</v>
@@ -14602,31 +14614,31 @@
         <v>0</v>
       </c>
       <c r="P21" s="123">
-        <v>11.955680293153282</v>
+        <v>20</v>
       </c>
       <c r="Q21" s="119">
         <v>0</v>
       </c>
       <c r="R21" s="119">
-        <v>1600.0000000000002</v>
+        <v>3200</v>
       </c>
       <c r="S21" s="124">
         <v>25</v>
       </c>
       <c r="T21" s="121">
-        <v>3345.6899999999946</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="22" ht="24" customHeight="1">
       <c r="A22" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="8" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E22" s="119">
         <v>0</v>
@@ -14641,19 +14653,19 @@
         <v>0</v>
       </c>
       <c r="I22" s="123">
-        <v>5.3067993366500845</v>
+        <v>5.296</v>
       </c>
       <c r="J22" s="119">
         <v>0</v>
       </c>
       <c r="K22" s="119">
-        <v>6400.0000000000009</v>
+        <v>6400</v>
       </c>
       <c r="L22" s="124">
         <v>12.5</v>
       </c>
       <c r="M22" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N22" s="125">
         <v>0.5</v>
@@ -14662,31 +14674,31 @@
         <v>0</v>
       </c>
       <c r="P22" s="123">
-        <v>23.911360586306564</v>
+        <v>20</v>
       </c>
       <c r="Q22" s="119">
         <v>0</v>
       </c>
       <c r="R22" s="119">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="S22" s="124">
         <v>25</v>
       </c>
       <c r="T22" s="121">
-        <v>3345.6899999999946</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="23" ht="24" customHeight="1">
       <c r="A23" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E23" s="119">
         <v>0</v>
@@ -14695,25 +14707,25 @@
         <v>0</v>
       </c>
       <c r="G23" s="121">
-        <v>80000</v>
+        <v>40000</v>
       </c>
       <c r="H23" s="122">
         <v>0</v>
       </c>
       <c r="I23" s="123">
-        <v>5.3067993366500845</v>
+        <v>2.648</v>
       </c>
       <c r="J23" s="119">
         <v>0</v>
       </c>
       <c r="K23" s="119">
-        <v>6400.0000000000009</v>
+        <v>3200</v>
       </c>
       <c r="L23" s="124">
         <v>12.5</v>
       </c>
       <c r="M23" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N23" s="125">
         <v>0.5</v>
@@ -14722,31 +14734,31 @@
         <v>0</v>
       </c>
       <c r="P23" s="123">
-        <v>23.911360586306564</v>
+        <v>10</v>
       </c>
       <c r="Q23" s="119">
         <v>0</v>
       </c>
       <c r="R23" s="119">
-        <v>3200.0000000000005</v>
+        <v>1600</v>
       </c>
       <c r="S23" s="124">
         <v>25</v>
       </c>
       <c r="T23" s="121">
-        <v>3345.6899999999946</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="24" ht="24" customHeight="1">
       <c r="A24" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E24" s="119">
         <v>0</v>
@@ -14761,19 +14773,19 @@
         <v>0</v>
       </c>
       <c r="I24" s="123">
-        <v>2.6533996683250423</v>
+        <v>2.648</v>
       </c>
       <c r="J24" s="119">
         <v>0</v>
       </c>
       <c r="K24" s="119">
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="L24" s="124">
         <v>12.5</v>
       </c>
       <c r="M24" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N24" s="125">
         <v>0.5</v>
@@ -14782,26 +14794,26 @@
         <v>0</v>
       </c>
       <c r="P24" s="123">
-        <v>11.955680293153282</v>
+        <v>10</v>
       </c>
       <c r="Q24" s="119">
         <v>0</v>
       </c>
       <c r="R24" s="119">
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="S24" s="124">
         <v>25</v>
       </c>
       <c r="T24" s="121">
-        <v>3345.6899999999946</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="25" ht="24" customHeight="1">
       <c r="B25" s="25"/>
       <c r="C25" s="39"/>
       <c r="D25" s="40" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E25" s="51">
         <v>0</v>
@@ -14816,19 +14828,19 @@
         <v>38</v>
       </c>
       <c r="I25" s="80">
-        <v>27.783667651535421</v>
+        <v>26.48</v>
       </c>
       <c r="J25" s="51" t="s">
         <v>38</v>
       </c>
       <c r="K25" s="51">
-        <v>32000.000000000004</v>
+        <v>32000</v>
       </c>
       <c r="L25" s="47">
         <v>12.5</v>
       </c>
       <c r="M25" s="43">
-        <v>14396.947336716898</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N25" s="45" t="s">
         <v>38</v>
@@ -14837,19 +14849,19 @@
         <v>38</v>
       </c>
       <c r="P25" s="80">
-        <v>119.55680293153282</v>
+        <v>100</v>
       </c>
       <c r="Q25" s="51" t="s">
         <v>38</v>
       </c>
       <c r="R25" s="51">
-        <v>16000.000000000002</v>
+        <v>16000</v>
       </c>
       <c r="S25" s="47">
         <v>25</v>
       </c>
       <c r="T25" s="43">
-        <v>3345.6899999999946</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="27" ht="24" customHeight="1">
@@ -14869,7 +14881,7 @@
       <c r="L27" s="139"/>
       <c r="M27" s="140"/>
       <c r="N27" s="138" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="O27" s="139"/>
       <c r="P27" s="139"/>
@@ -14880,14 +14892,14 @@
     </row>
     <row r="28" ht="24" customHeight="1">
       <c r="A28" s="99" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>23</v>
@@ -14940,14 +14952,14 @@
     </row>
     <row r="29" ht="24" customHeight="1">
       <c r="A29" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E29" s="119">
         <v>0</v>
@@ -14962,7 +14974,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="123">
-        <v>14.516669309910206</v>
+        <v>13.240000000000002</v>
       </c>
       <c r="J29" s="119">
         <v>0</v>
@@ -14974,7 +14986,7 @@
         <v>12.5</v>
       </c>
       <c r="M29" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N29" s="125">
         <v>0.5</v>
@@ -14983,7 +14995,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="123">
-        <v>59.7784014657664</v>
+        <v>50</v>
       </c>
       <c r="Q29" s="119">
         <v>0</v>
@@ -14995,19 +15007,19 @@
         <v>25</v>
       </c>
       <c r="T29" s="121">
-        <v>3345.69</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="30" ht="24" customHeight="1">
       <c r="A30" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E30" s="119">
         <v>0</v>
@@ -15022,7 +15034,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="123">
-        <v>14.516669309910206</v>
+        <v>13.240000000000002</v>
       </c>
       <c r="J30" s="119">
         <v>0</v>
@@ -15034,7 +15046,7 @@
         <v>12.5</v>
       </c>
       <c r="M30" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N30" s="125">
         <v>0.5</v>
@@ -15043,7 +15055,7 @@
         <v>0</v>
       </c>
       <c r="P30" s="123">
-        <v>59.7784014657664</v>
+        <v>50</v>
       </c>
       <c r="Q30" s="119">
         <v>0</v>
@@ -15055,19 +15067,19 @@
         <v>25</v>
       </c>
       <c r="T30" s="121">
-        <v>3345.69</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="31" ht="24" customHeight="1">
       <c r="A31" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E31" s="119">
         <v>0</v>
@@ -15076,25 +15088,25 @@
         <v>0</v>
       </c>
       <c r="G31" s="121">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="H31" s="122">
         <v>0</v>
       </c>
       <c r="I31" s="123">
-        <v>7.2583346549551031</v>
+        <v>13.240000000000002</v>
       </c>
       <c r="J31" s="119">
         <v>0</v>
       </c>
       <c r="K31" s="119">
-        <v>8000</v>
+        <v>16000</v>
       </c>
       <c r="L31" s="124">
         <v>12.5</v>
       </c>
       <c r="M31" s="121">
-        <v>13777.265000000005</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N31" s="125">
         <v>0.5</v>
@@ -15103,31 +15115,31 @@
         <v>0</v>
       </c>
       <c r="P31" s="123">
-        <v>29.8892007328832</v>
+        <v>50</v>
       </c>
       <c r="Q31" s="119">
         <v>0</v>
       </c>
       <c r="R31" s="119">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="S31" s="124">
         <v>25</v>
       </c>
       <c r="T31" s="121">
-        <v>3345.69</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="32" ht="24" customHeight="1">
       <c r="A32" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="8" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E32" s="119">
         <v>0</v>
@@ -15142,7 +15154,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="123">
-        <v>13.266998341625209</v>
+        <v>13.240000000000002</v>
       </c>
       <c r="J32" s="119">
         <v>0</v>
@@ -15154,7 +15166,7 @@
         <v>12.5</v>
       </c>
       <c r="M32" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N32" s="125">
         <v>0.5</v>
@@ -15163,7 +15175,7 @@
         <v>0</v>
       </c>
       <c r="P32" s="123">
-        <v>59.7784014657664</v>
+        <v>50</v>
       </c>
       <c r="Q32" s="119">
         <v>0</v>
@@ -15175,19 +15187,19 @@
         <v>25</v>
       </c>
       <c r="T32" s="121">
-        <v>3345.69</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="33" ht="24" customHeight="1">
       <c r="A33" s="99" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E33" s="119">
         <v>0</v>
@@ -15196,25 +15208,25 @@
         <v>0</v>
       </c>
       <c r="G33" s="121">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="H33" s="122">
         <v>0</v>
       </c>
       <c r="I33" s="123">
-        <v>13.266998341625209</v>
+        <v>6.620000000000001</v>
       </c>
       <c r="J33" s="119">
         <v>0</v>
       </c>
       <c r="K33" s="119">
-        <v>16000</v>
+        <v>8000</v>
       </c>
       <c r="L33" s="124">
         <v>12.5</v>
       </c>
       <c r="M33" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N33" s="125">
         <v>0.5</v>
@@ -15223,31 +15235,31 @@
         <v>0</v>
       </c>
       <c r="P33" s="123">
-        <v>59.7784014657664</v>
+        <v>25</v>
       </c>
       <c r="Q33" s="119">
         <v>0</v>
       </c>
       <c r="R33" s="119">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="S33" s="124">
         <v>25</v>
       </c>
       <c r="T33" s="121">
-        <v>3345.69</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="34" ht="24" customHeight="1">
       <c r="A34" s="99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B34" s="25"/>
       <c r="C34" s="8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E34" s="119">
         <v>0</v>
@@ -15262,7 +15274,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="123">
-        <v>6.6334991708126045</v>
+        <v>6.620000000000001</v>
       </c>
       <c r="J34" s="119">
         <v>0</v>
@@ -15274,7 +15286,7 @@
         <v>12.5</v>
       </c>
       <c r="M34" s="121">
-        <v>15075.000000000009</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N34" s="125">
         <v>0.5</v>
@@ -15283,7 +15295,7 @@
         <v>0</v>
       </c>
       <c r="P34" s="123">
-        <v>29.8892007328832</v>
+        <v>25</v>
       </c>
       <c r="Q34" s="119">
         <v>0</v>
@@ -15295,14 +15307,14 @@
         <v>25</v>
       </c>
       <c r="T34" s="121">
-        <v>3345.69</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="35" ht="24" customHeight="1">
       <c r="B35" s="25"/>
       <c r="C35" s="39"/>
       <c r="D35" s="40" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E35" s="51">
         <v>0</v>
@@ -15317,7 +15329,7 @@
         <v>38</v>
       </c>
       <c r="I35" s="80">
-        <v>69.459169128838539</v>
+        <v>66.200000000000017</v>
       </c>
       <c r="J35" s="51" t="s">
         <v>38</v>
@@ -15329,7 +15341,7 @@
         <v>12.5</v>
       </c>
       <c r="M35" s="43">
-        <v>14396.947336716898</v>
+        <v>15105.740181268882</v>
       </c>
       <c r="N35" s="45" t="s">
         <v>38</v>
@@ -15338,7 +15350,7 @@
         <v>38</v>
       </c>
       <c r="P35" s="80">
-        <v>298.892007328832</v>
+        <v>250</v>
       </c>
       <c r="Q35" s="51" t="s">
         <v>38</v>
@@ -15350,7 +15362,7 @@
         <v>25</v>
       </c>
       <c r="T35" s="43">
-        <v>3345.69</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="37" ht="48" customHeight="1">
@@ -15360,7 +15372,7 @@
       <c r="D37" s="55"/>
       <c r="E37" s="117"/>
       <c r="F37" s="145" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G37" s="145"/>
       <c r="H37" s="145"/>
@@ -15485,7 +15497,7 @@
       </c>
       <c r="D43" s="55"/>
       <c r="F43" s="145" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G43" s="145"/>
       <c r="H43" s="145"/>
@@ -15527,7 +15539,7 @@
       </c>
       <c r="D45" s="55"/>
       <c r="F45" s="136" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G45" s="136"/>
       <c r="H45" s="136"/>
@@ -15546,6 +15558,11 @@
     </row>
   </sheetData>
   <mergeCells>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="F39:T39"/>
     <mergeCell ref="F41:T41"/>
     <mergeCell ref="F43:T43"/>
     <mergeCell ref="F45:T45"/>
@@ -15555,11 +15572,6 @@
     <mergeCell ref="H7:M7"/>
     <mergeCell ref="N7:T7"/>
     <mergeCell ref="F37:T37"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F39:T39"/>
     <mergeCell ref="H17:M17"/>
     <mergeCell ref="N17:T17"/>
     <mergeCell ref="H27:M27"/>

</xml_diff>